<commit_message>
Update BBM upload log
</commit_message>
<xml_diff>
--- a/data/bbm_upload_log.xlsx
+++ b/data/bbm_upload_log.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>BBM_STD</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>2025-12-02 11:38</t>
+  </si>
+  <si>
+    <t>2025-12-02 11:39</t>
   </si>
   <si>
     <t>2025-12</t>
@@ -401,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -438,7 +441,24 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>